<commit_message>
Diccionario de datos y diagrama workbench
Faltaba de actualizar jejeje
</commit_message>
<xml_diff>
--- a/Documentación/Diccionario de datos.xlsx
+++ b/Documentación/Diccionario de datos.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reymi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerardo GC\Documents\Farmacia\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CB54F5-42E1-485B-844D-E1239620FADC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="602" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" tabRatio="602" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Proveedor" sheetId="3" r:id="rId1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="102">
   <si>
     <t>Campo</t>
   </si>
@@ -56,9 +55,6 @@
     <t>INT</t>
   </si>
   <si>
-    <t>Registro fereral de contribuyentes</t>
-  </si>
-  <si>
     <t>Nombre del empleado</t>
   </si>
   <si>
@@ -83,9 +79,6 @@
     <t>Nombre</t>
   </si>
   <si>
-    <t>RFC</t>
-  </si>
-  <si>
     <t>Telefono</t>
   </si>
   <si>
@@ -185,9 +178,6 @@
     <t>Clave única de los empleados</t>
   </si>
   <si>
-    <t>Clave única del empleado</t>
-  </si>
-  <si>
     <t>Clave única del producto</t>
   </si>
   <si>
@@ -281,9 +271,6 @@
     <t>Referencia a la Compra</t>
   </si>
   <si>
-    <t>Referencia hacia el cliente</t>
-  </si>
-  <si>
     <t>idPromocion</t>
   </si>
   <si>
@@ -332,20 +319,35 @@
     <t>Precio_compra</t>
   </si>
   <si>
-    <t>double</t>
-  </si>
-  <si>
     <t>Precio para la venta publica</t>
   </si>
   <si>
     <t>Precio para la compra del proveedor</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>DOUBLE</t>
+  </si>
+  <si>
+    <t>Total del producto</t>
+  </si>
+  <si>
+    <t>Cantidad del producto</t>
+  </si>
+  <si>
+    <t>Promocion</t>
+  </si>
+  <si>
+    <t>Referencia a la promoción</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -724,21 +726,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="11"/>
-    <col min="4" max="4" width="29.5703125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="11" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" style="11"/>
+    <col min="4" max="4" width="29.5546875" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30">
+    <row r="1" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -752,89 +754,89 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="4">
+        <v>100</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="B3" s="4">
-        <v>50</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="B4" s="4">
         <v>20</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="4">
+        <v>45</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" s="1">
-        <v>45</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" s="1">
+      <c r="B6" s="4">
         <v>120</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="C6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="2"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
@@ -846,21 +848,21 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -874,88 +876,102 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75">
+    <row r="2" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75">
-      <c r="A4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75">
-      <c r="A5" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A4" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.4">
+      <c r="A5" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A6" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.4">
+      <c r="A7" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="D6" s="16" t="s">
+      <c r="B7" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="16" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30.75">
-      <c r="A7" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" s="7" t="s">
+    <row r="8" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.4">
+      <c r="A8" s="16" t="s">
         <v>100</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -964,21 +980,21 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="24.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -992,32 +1008,32 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30">
+    <row r="2" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="30">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1026,21 +1042,21 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" customWidth="1"/>
+    <col min="4" max="4" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1054,46 +1070,46 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75">
+    <row r="2" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="6">
         <v>120</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A4" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1102,20 +1118,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="4" max="4" width="24.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1129,60 +1145,60 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="34.9" customHeight="1">
+    <row r="2" spans="1:4" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="30">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="54.6" customHeight="1">
+    </row>
+    <row r="4" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="45">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1191,22 +1207,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1220,60 +1236,60 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1282,22 +1298,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J5" sqref="J4:J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30">
+    <row r="1" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1311,32 +1327,32 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30">
+    <row r="2" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="30">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="4">
         <v>45</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1345,23 +1361,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="35.7109375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.5703125" style="1"/>
+    <col min="1" max="1" width="16.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="35.6640625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1375,165 +1391,166 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="4" t="s">
+      <c r="B3" s="4">
+        <v>50</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="4">
-        <v>20</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="14.45" customHeight="1">
-      <c r="A4" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="B4" s="4">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4">
         <v>50</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="30">
-      <c r="A7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="4" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30">
-      <c r="A8" s="4" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="B9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" s="4">
+        <v>100</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.5546875" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" customWidth="1"/>
+    <col min="4" max="4" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1547,35 +1564,35 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30">
+    <row r="2" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="30">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="10">
         <v>100</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C8" s="15"/>
     </row>
   </sheetData>
@@ -1584,21 +1601,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="11.5703125" style="13"/>
-    <col min="4" max="4" width="26.85546875" style="13" customWidth="1"/>
-    <col min="5" max="16384" width="11.5703125" style="13"/>
+    <col min="1" max="3" width="11.5546875" style="13"/>
+    <col min="4" max="4" width="26.88671875" style="13" customWidth="1"/>
+    <col min="5" max="16384" width="11.5546875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1612,51 +1629,51 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="10">
         <v>100</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B4" s="10">
         <v>120</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" s="10">
         <v>20</v>
@@ -1665,12 +1682,12 @@
         <v>5</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B6" s="10">
         <v>5</v>
@@ -1679,40 +1696,40 @@
         <v>5</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="45">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E7" s="14"/>
     </row>
-    <row r="8" spans="1:5" ht="30">
+    <row r="8" spans="1:5" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B8" s="10">
         <v>45</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E8" s="14"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1725,23 +1742,23 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="5"/>
-    <col min="3" max="3" width="12.28515625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="38.140625" style="8" customWidth="1"/>
-    <col min="5" max="16384" width="11.5703125" style="5"/>
+    <col min="1" max="1" width="13.6640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" style="5"/>
+    <col min="3" max="3" width="12.33203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="38.109375" style="8" customWidth="1"/>
+    <col min="5" max="16384" width="11.5546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="34.9" customHeight="1">
+    <row r="1" spans="1:4" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1755,104 +1772,91 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="30">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="7">
         <v>100</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="7">
+        <v>45</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="30">
-      <c r="A4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="7">
-        <v>20</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="7" t="s">
+      <c r="D5" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="30">
-      <c r="A6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="7">
-        <v>45</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>8</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>10</v>
+    <row r="7" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A7" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>5</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="30">
-      <c r="A8" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.4"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1860,20 +1864,20 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1887,69 +1891,77 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75">
+    <row r="2" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.4">
+      <c r="A3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75">
-      <c r="A3" s="6" t="s">
+    </row>
+    <row r="4" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.4">
+      <c r="A4" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75">
-      <c r="A4" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="B4" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-    </row>
-    <row r="7" spans="1:4" ht="15.75">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.4">
+      <c r="A6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>

</xml_diff>